<commit_message>
retti retti meget pis
</commit_message>
<xml_diff>
--- a/Assets/Excel Budget/a.xlsx
+++ b/Assets/Excel Budget/a.xlsx
@@ -1,21 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Maj</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>båd</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Okt</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Udgifter</t>
+  </si>
+  <si>
+    <t>Indtægter</t>
+  </si>
+  <si>
+    <t>øvrige udgifter</t>
+  </si>
+  <si>
+    <t>øvrige indtægter</t>
+  </si>
+  <si>
+    <t>overført fra</t>
+  </si>
+  <si>
+    <t>opsparing</t>
+  </si>
+  <si>
+    <t>ulykke</t>
+  </si>
+  <si>
+    <t>energi nord</t>
+  </si>
+  <si>
+    <t>vandafgift</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +402,439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>17500</v>
+      </c>
+      <c r="C4">
+        <v>17500</v>
+      </c>
+      <c r="D4">
+        <v>17500</v>
+      </c>
+      <c r="E4">
+        <v>17500</v>
+      </c>
+      <c r="F4">
+        <v>17500</v>
+      </c>
+      <c r="G4">
+        <v>17500</v>
+      </c>
+      <c r="H4">
+        <v>17500</v>
+      </c>
+      <c r="I4">
+        <v>17500</v>
+      </c>
+      <c r="J4">
+        <v>17500</v>
+      </c>
+      <c r="K4">
+        <v>17500</v>
+      </c>
+      <c r="L4">
+        <v>17500</v>
+      </c>
+      <c r="M4">
+        <v>17500</v>
+      </c>
+      <c r="N4">
+        <f>SUM(B4:M4)</f>
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>17500</v>
+      </c>
+      <c r="C5">
+        <v>17500</v>
+      </c>
+      <c r="D5">
+        <v>17500</v>
+      </c>
+      <c r="E5">
+        <v>17500</v>
+      </c>
+      <c r="F5">
+        <v>17500</v>
+      </c>
+      <c r="G5">
+        <v>17500</v>
+      </c>
+      <c r="H5">
+        <v>17500</v>
+      </c>
+      <c r="I5">
+        <v>17500</v>
+      </c>
+      <c r="J5">
+        <v>17500</v>
+      </c>
+      <c r="K5">
+        <v>17500</v>
+      </c>
+      <c r="L5">
+        <v>17500</v>
+      </c>
+      <c r="M5">
+        <v>17500</v>
+      </c>
+      <c r="N5">
+        <f>SUM(B5:M5)</f>
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>11</v>
+      </c>
+      <c r="M12">
+        <v>12</v>
+      </c>
+      <c r="N12">
+        <f>SUM(B12:M12)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ref="N13:N17" si="0">SUM(B13:M13)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>11</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>11</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16">
+        <v>10</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>12</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>SUM(B12:B16)</f>
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:M17" si="1">SUM(C12:C16)</f>
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
penge-puling (hårdt) af mr lister the sister fister
</commit_message>
<xml_diff>
--- a/Assets/Excel Budget/a.xlsx
+++ b/Assets/Excel Budget/a.xlsx
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tape fixed  HAR ÆNDRET EXCEL A SÅ DET IKKE VIRKER LÆNGERE ÆNDRE EXCEL TIL AT DER ER NOGET HVER MÅNED
</commit_message>
<xml_diff>
--- a/Assets/Excel Budget/a.xlsx
+++ b/Assets/Excel Budget/a.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,44 +560,26 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>2000</v>
-      </c>
-      <c r="C12">
-        <v>2000</v>
+        <v>2038</v>
       </c>
       <c r="D12">
-        <v>2000</v>
-      </c>
-      <c r="E12">
-        <v>2000</v>
+        <v>2038</v>
       </c>
       <c r="F12">
-        <v>2000</v>
-      </c>
-      <c r="G12">
-        <v>2000</v>
+        <v>2038</v>
       </c>
       <c r="H12">
-        <v>2000</v>
-      </c>
-      <c r="I12">
-        <v>2000</v>
+        <v>2038</v>
       </c>
       <c r="J12">
-        <v>2000</v>
-      </c>
-      <c r="K12">
-        <v>2000</v>
+        <v>2038</v>
       </c>
       <c r="L12">
-        <v>2000</v>
-      </c>
-      <c r="M12">
-        <v>2000</v>
+        <v>2038</v>
       </c>
       <c r="N12">
         <f>SUM(B12:M12)</f>
-        <v>24000</v>
+        <v>12228</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -605,44 +587,44 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="C13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="D13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="E13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="F13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="G13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="H13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="I13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="J13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="K13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="L13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="M13">
-        <v>1555</v>
+        <v>1149</v>
       </c>
       <c r="N13">
         <f t="shared" ref="N13:N17" si="0">SUM(B13:M13)</f>
-        <v>18660</v>
+        <v>13788</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -694,86 +676,26 @@
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
-        <v>10500</v>
-      </c>
       <c r="C15">
         <v>10500</v>
       </c>
-      <c r="D15">
-        <v>10500</v>
-      </c>
-      <c r="E15">
-        <v>10500</v>
-      </c>
       <c r="F15">
         <v>10500</v>
       </c>
-      <c r="G15">
-        <v>10500</v>
-      </c>
-      <c r="H15">
-        <v>10500</v>
-      </c>
       <c r="I15">
         <v>10500</v>
       </c>
-      <c r="J15">
-        <v>10500</v>
-      </c>
-      <c r="K15">
-        <v>10500</v>
-      </c>
       <c r="L15">
         <v>10500</v>
-      </c>
-      <c r="M15">
-        <v>10500</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="0"/>
-        <v>126000</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
-        <v>750</v>
-      </c>
-      <c r="C16">
-        <v>750</v>
-      </c>
-      <c r="D16">
-        <v>750</v>
-      </c>
-      <c r="E16">
-        <v>750</v>
-      </c>
-      <c r="F16">
-        <v>750</v>
-      </c>
-      <c r="G16">
-        <v>750</v>
-      </c>
-      <c r="H16">
-        <v>750</v>
-      </c>
-      <c r="I16">
-        <v>750</v>
-      </c>
-      <c r="J16">
-        <v>750</v>
-      </c>
-      <c r="K16">
-        <v>750</v>
-      </c>
       <c r="L16">
-        <v>750</v>
-      </c>
-      <c r="M16">
-        <v>750</v>
+        <f>750*12</f>
+        <v>9000</v>
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
@@ -783,55 +705,55 @@
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>SUM(B12:B16)</f>
-        <v>15471</v>
+        <v>3853</v>
       </c>
       <c r="C17">
         <f t="shared" ref="C17:M17" si="1">SUM(C12:C16)</f>
-        <v>15471</v>
+        <v>12315</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>3853</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>1815</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>14353</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>1815</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>3853</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>12315</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>3853</v>
       </c>
       <c r="K17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>1815</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>23353</v>
       </c>
       <c r="M17">
         <f t="shared" si="1"/>
-        <v>15471</v>
+        <v>1815</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>185652</v>
+        <v>85008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>